<commit_message>
updates levels in recapture metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_recapture_metadata.xlsx
+++ b/data-raw/metadata/feather_recapture_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-feather-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C3C942-AE71-EF4B-B57B-930E223B58FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{701BD459-587A-B244-B578-A00C84C3436B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31940" yWindow="-21000" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -100,16 +100,10 @@
     <t>commonName</t>
   </si>
   <si>
-    <t>Common name of species</t>
-  </si>
-  <si>
     <t>releaseID</t>
   </si>
   <si>
     <t>Foreign Key to the CAMP Release table</t>
-  </si>
-  <si>
-    <t>Run as assigned at the time of the capture.</t>
   </si>
   <si>
     <t>fishOrigin</t>
@@ -208,15 +202,6 @@
     <t>markCode</t>
   </si>
   <si>
-    <t>type of mark on fish</t>
-  </si>
-  <si>
-    <t>color of mark on fish</t>
-  </si>
-  <si>
-    <t>position of mark on body of fish</t>
-  </si>
-  <si>
     <t>code identifying the type of mark</t>
   </si>
   <si>
@@ -236,6 +221,21 @@
   </si>
   <si>
     <t>Name of the trap or trap location. Levels = c("Eye riffle_north", "Herringer_west", "Herringer_east", "#Steep Riffle_RST", "Sunset West bank", "Sunset East bank", "Gateway_main1", "Live Oak", "Eye riffle_Side Channel", "Herringer_Upper_west", "Steep Riffle_10' ext", "Gateway Main 400' Up River", "Gateway_Rootball")</t>
+  </si>
+  <si>
+    <t>Common name of species. Levels = "Chinook salmon"</t>
+  </si>
+  <si>
+    <t>Run as assigned at the time of the capture. Levels = c("Not recorded", "Fall", "Spring")</t>
+  </si>
+  <si>
+    <t>type of mark on fish. Levels = c("Elastomer", "Pigment / dye", "Fin clip")</t>
+  </si>
+  <si>
+    <t>color of mark on fish. Levels = c("White", "Brown", "Orange", "Green", "Red", "Blue", "yellow", "Purple / Violet", "Pink", "Not applicable (n/a)", "Fluorescent red", "Fluorescent blue")</t>
+  </si>
+  <si>
+    <t>position of mark on body of fish. Levels = c("Nose", "Wholte body", "Adipose fin", "Not recorded")</t>
   </si>
 </sst>
 </file>
@@ -625,7 +625,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>14</v>
@@ -739,7 +739,7 @@
         <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>14</v>
@@ -774,10 +774,10 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>19</v>
@@ -812,10 +812,10 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>14</v>
@@ -850,10 +850,10 @@
     </row>
     <row r="8" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>14</v>
@@ -888,10 +888,10 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>14</v>
@@ -926,10 +926,10 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>14</v>
@@ -964,28 +964,28 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G11" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="H11" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="3"/>
@@ -1008,28 +1008,28 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="H12" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="3"/>
@@ -1052,26 +1052,26 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="3"/>
@@ -1094,10 +1094,10 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>14</v>
@@ -1132,26 +1132,26 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="I15" s="6"/>
       <c r="J15" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K15" s="6"/>
       <c r="L15" s="5"/>
@@ -1172,10 +1172,10 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>14</v>
@@ -1210,10 +1210,10 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>14</v>
@@ -1248,10 +1248,10 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>14</v>
@@ -1286,10 +1286,10 @@
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>14</v>
@@ -1324,10 +1324,10 @@
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>14</v>
@@ -1362,10 +1362,10 @@
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>14</v>
@@ -1400,10 +1400,10 @@
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>14</v>
@@ -28470,13 +28470,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>

</xml_diff>

<commit_message>
creates methods.md to format method doc. validates xml
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_recapture_metadata.xlsx
+++ b/data-raw/metadata/feather_recapture_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-feather-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACEA6190-6F90-3044-A8BD-456B83BB3D68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A000603-B094-3349-9240-E23D75CEB22B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9060" yWindow="-20340" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>nominal</t>
-  </si>
-  <si>
-    <t>catch</t>
   </si>
   <si>
     <t>catchRawID</t>
@@ -242,6 +239,9 @@
   </si>
   <si>
     <t>Feather River RST program</t>
+  </si>
+  <si>
+    <t>recapture</t>
   </si>
 </sst>
 </file>
@@ -556,7 +556,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N12" sqref="N12"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -635,16 +635,16 @@
         <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -670,19 +670,19 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -708,19 +708,19 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -746,19 +746,19 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -784,19 +784,19 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -822,19 +822,19 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -860,19 +860,19 @@
     </row>
     <row r="8" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
@@ -898,19 +898,19 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -936,19 +936,19 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -974,28 +974,28 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="F11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="3"/>
@@ -1022,28 +1022,28 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>37</v>
+      <c r="C12" s="1" t="s">
+        <v>32</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="F12" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="3"/>
@@ -1070,28 +1070,28 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>39</v>
+      <c r="C13" s="1" t="s">
+        <v>32</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="F13" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="3"/>
@@ -1118,19 +1118,19 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -1156,26 +1156,26 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D15" s="2" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="I15" s="6"/>
       <c r="J15" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K15" s="6"/>
       <c r="L15" s="11">
@@ -1200,19 +1200,19 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
@@ -1238,19 +1238,19 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -1276,19 +1276,19 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -1314,19 +1314,19 @@
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -1352,19 +1352,19 @@
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -1390,19 +1390,19 @@
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
@@ -1428,19 +1428,19 @@
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -28498,13 +28498,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="10" t="s">
         <v>58</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>59</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -28535,7 +28535,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>13</v>

</xml_diff>